<commit_message>
DataTable 에 CONST 기능 추가. ㄴ커밋 누락된 WorkBook 적용. ㄴ itemDataTable 에 Const 로드 기능 추가.
</commit_message>
<xml_diff>
--- a/DataTable/Common/ItemDataTable.xlsx
+++ b/DataTable/Common/ItemDataTable.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1000Download\ProjectD\DataTable\Common\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23B6E5D3-1DAA-47F7-A585-521FE63E80C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF50EA7A-34DD-4D87-9692-C040CBAF8F08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="3060" windowWidth="20925" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26625" yWindow="5280" windowWidth="20925" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ITEM" sheetId="4" r:id="rId1"/>
+    <sheet name="CONST" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>SWORD</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -72,6 +73,18 @@
   </si>
   <si>
     <t>SPRITE_NAME</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>;피로도 1을 회복시킬 떄 필요한 시간.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CONST_FATIGUE_RECOVER_TIME</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>단위 : 초</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -79,7 +92,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -94,6 +107,12 @@
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF172B4D"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -118,9 +137,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -404,7 +429,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -480,4 +505,37 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75227B14-FDE7-4D8D-A249-DD45C69A473C}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="36.875" customWidth="1"/>
+    <col min="2" max="2" width="14.125" customWidth="1"/>
+    <col min="3" max="3" width="80.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1">
+        <v>160</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>